<commit_message>
added Rob update file to sandbox until able to review diff ; started ODD writing and finished ODD prep spreadsheet
</commit_message>
<xml_diff>
--- a/ODD_Schema/tei_conceptual_modeling_worksheet.xlsx
+++ b/ODD_Schema/tei_conceptual_modeling_worksheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="159">
   <si>
     <t>Feature</t>
   </si>
@@ -69,9 +69,6 @@
     <t>graphic</t>
   </si>
   <si>
-    <t xml:space="preserve"> url="RELATIVE IMAGE FILE NAME.fileExt"</t>
-  </si>
-  <si>
     <t>provides direct link to the related image for the previous page division</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>list</t>
   </si>
   <si>
-    <t>type="entry"</t>
-  </si>
-  <si>
     <t>division of grouped line entries</t>
   </si>
   <si>
@@ -183,9 +177,6 @@
     <t>type="first" type="middle" type="maiden"</t>
   </si>
   <si>
-    <t xml:space="preserve">generational name component; ie. Jr or II </t>
-  </si>
-  <si>
     <t>alias or nicknames</t>
   </si>
   <si>
@@ -237,9 +228,6 @@
     <t>geo</t>
   </si>
   <si>
-    <t>white-space separated lat. and long. coordinates; ie. 51.969604 -2.893146</t>
-  </si>
-  <si>
     <t xml:space="preserve">semantic markup </t>
   </si>
   <si>
@@ -267,12 +255,6 @@
     <t>may contain &lt;unclear&gt;</t>
   </si>
   <si>
-    <t>when="ISOstandard xxxx-xx-xx"</t>
-  </si>
-  <si>
-    <t>contains date text as appears on manuscript (ie. February 10 1802)</t>
-  </si>
-  <si>
     <t>g</t>
   </si>
   <si>
@@ -282,9 +264,6 @@
     <t>indicates unique character in manuscript text</t>
   </si>
   <si>
-    <t>slef-closing element</t>
-  </si>
-  <si>
     <t>gaiji</t>
   </si>
   <si>
@@ -310,6 +289,213 @@
   </si>
   <si>
     <t xml:space="preserve">signature like after name of person </t>
+  </si>
+  <si>
+    <t>sic</t>
+  </si>
+  <si>
+    <t>reg</t>
+  </si>
+  <si>
+    <t>unclear</t>
+  </si>
+  <si>
+    <t>add</t>
+  </si>
+  <si>
+    <t>reason="illegible | strikethrough" unit="words | chars" quantity="#ofUnit"</t>
+  </si>
+  <si>
+    <t>supplied</t>
+  </si>
+  <si>
+    <t>semantic markup</t>
+  </si>
+  <si>
+    <t>must appear in &lt;unclear&gt; element</t>
+  </si>
+  <si>
+    <t>indicates text that cannot be described (gives reason and number of missing words or characters</t>
+  </si>
+  <si>
+    <t>choice</t>
+  </si>
+  <si>
+    <t>surrounds word with odd spelling that is in manuscript</t>
+  </si>
+  <si>
+    <t>regularized spelling of previous word with odd spelling</t>
+  </si>
+  <si>
+    <t>contains words from amnuscript that have odd spelling and the modern, normal spelling</t>
+  </si>
+  <si>
+    <t>must contain &lt;sic&gt; and &lt;reg&gt;</t>
+  </si>
+  <si>
+    <t>must be within &lt;choice&gt; and come before &lt;reg&gt;</t>
+  </si>
+  <si>
+    <t>must be within &lt;choice&gt; and come after &lt;sic&gt;</t>
+  </si>
+  <si>
+    <t>used when transcription is unsure; contains educated guess at manuscript text</t>
+  </si>
+  <si>
+    <t>provides missing text when manuscript indicates (ex. when ditto character is used)</t>
+  </si>
+  <si>
+    <t>should appear after &lt;g ref="#ditto"/&gt; ??</t>
+  </si>
+  <si>
+    <t>type="entry" subtype="total"(used only if the line items indicate total cost/price/summary)</t>
+  </si>
+  <si>
+    <t>self-closing element</t>
+  </si>
+  <si>
+    <t>must be self closing or contain &lt;supplied&gt;  and cannot be followed by another &lt;unclear&gt; element</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generational name component; i.e. Jr or II </t>
+  </si>
+  <si>
+    <t>white-space separated lat. and long. coordinates; i.e. 51.969604 -2.893146</t>
+  </si>
+  <si>
+    <t>contains date text as appears on manuscript (i.e. February 10 1802)</t>
+  </si>
+  <si>
+    <t>url="RELATIVE IMAGE FILE NAME.fileExt"</t>
+  </si>
+  <si>
+    <t>when="ISOstandard xxxx-xx-xx or xxxx-xx or xxxx"</t>
+  </si>
+  <si>
+    <t>from-iso="ISOstandard" to-iso="1819"</t>
+  </si>
+  <si>
+    <t>transcr</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>authority</t>
+  </si>
+  <si>
+    <t>availability</t>
+  </si>
+  <si>
+    <t>char</t>
+  </si>
+  <si>
+    <t>header</t>
+  </si>
+  <si>
+    <t>charDecl</t>
+  </si>
+  <si>
+    <t>charName</t>
+  </si>
+  <si>
+    <t>collection</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>desc</t>
+  </si>
+  <si>
+    <t>edition</t>
+  </si>
+  <si>
+    <t>editionStmt</t>
+  </si>
+  <si>
+    <t>editorialDecl</t>
+  </si>
+  <si>
+    <t>encodingDesc</t>
+  </si>
+  <si>
+    <t>figure</t>
+  </si>
+  <si>
+    <t>msDesc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">msdescription </t>
+  </si>
+  <si>
+    <t>header </t>
+  </si>
+  <si>
+    <t>fileDesc</t>
+  </si>
+  <si>
+    <t>figures</t>
+  </si>
+  <si>
+    <t>handNote</t>
+  </si>
+  <si>
+    <t>handNotes</t>
+  </si>
+  <si>
+    <t>idno</t>
+  </si>
+  <si>
+    <t>license</t>
+  </si>
+  <si>
+    <t>msIdentifier</t>
+  </si>
+  <si>
+    <t>orgName</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>physDesc</t>
+  </si>
+  <si>
+    <t>placeName</t>
+  </si>
+  <si>
+    <t>principal</t>
+  </si>
+  <si>
+    <t>profileDesc</t>
+  </si>
+  <si>
+    <t>pubPlace</t>
+  </si>
+  <si>
+    <t>publicationStmt</t>
+  </si>
+  <si>
+    <t>repository</t>
+  </si>
+  <si>
+    <t>resp</t>
+  </si>
+  <si>
+    <t>respStmt</t>
+  </si>
+  <si>
+    <t>sourceDesc</t>
+  </si>
+  <si>
+    <t>sponsor</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>titleStmt</t>
   </si>
 </sst>
 </file>
@@ -655,20 +841,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z33"/>
+  <dimension ref="A1:Z79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C27" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="D32" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.5703125" customWidth="1"/>
     <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="48" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="74.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="77.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="83.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="75.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="83.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -716,209 +902,226 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
+      <c r="C4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>20</v>
+        <v>109</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>12</v>
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="D7" s="4" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" t="s">
-        <v>18</v>
+        <v>35</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>36</v>
+        <v>41</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>12</v>
+        <v>43</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="F13" s="4" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="B14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="B15" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="D15" t="s">
+        <v>112</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -926,243 +1129,783 @@
         <v>49</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D17" t="s">
+      <c r="C17" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>54</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="B18" s="4" t="s">
-        <v>51</v>
+        <v>56</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="B19" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>18</v>
+        <v>40</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
+      </c>
+      <c r="D22" t="s">
+        <v>113</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>42</v>
+      <c r="D25" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="D26" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E26" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>79</v>
-      </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>74</v>
-      </c>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
       <c r="C27" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>79</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B28" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="E28" t="s">
+        <v>81</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C29" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E29" t="s">
-        <v>88</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C30" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C31" s="4" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C32" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>90</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>96</v>
+      </c>
+      <c r="B36" t="s">
         <v>91</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="C36" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E36" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>96</v>
+      </c>
+      <c r="B37" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" t="s">
+        <v>94</v>
+      </c>
+      <c r="D37" t="s">
+        <v>98</v>
+      </c>
+      <c r="E37" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>96</v>
+      </c>
+      <c r="B38" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="33" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C33" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D33" s="4" t="s">
+      <c r="C38" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F38" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>96</v>
+      </c>
+      <c r="B39" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E39" t="s">
+        <v>17</v>
+      </c>
+      <c r="F39" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+    </row>
+    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E51" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E52" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E53" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E54" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E56" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to ODD -- defined attributes, accounted for graphic in div, started writing schema rule (getting an error on choice?); pulled RF changes to transcriptions into sandbox for later review; made additions to ODD prep spreadsheet
</commit_message>
<xml_diff>
--- a/ODD_Schema/tei_conceptual_modeling_worksheet.xlsx
+++ b/ODD_Schema/tei_conceptual_modeling_worksheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="162">
   <si>
     <t>Feature</t>
   </si>
@@ -51,9 +51,6 @@
     <t>div</t>
   </si>
   <si>
-    <t>type="page"</t>
-  </si>
-  <si>
     <t>division based off of the manuscript page divisions</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
     <t>core</t>
   </si>
   <si>
-    <t>self-closing and contained by div</t>
-  </si>
-  <si>
     <t>type="group"</t>
   </si>
   <si>
@@ -496,6 +490,21 @@
   </si>
   <si>
     <t>titleStmt</t>
+  </si>
+  <si>
+    <t>facimile</t>
+  </si>
+  <si>
+    <t>self-closing and contained by facimile which is contained by div</t>
+  </si>
+  <si>
+    <t>contained by div; contains graphic</t>
+  </si>
+  <si>
+    <t>indicates representation of original document</t>
+  </si>
+  <si>
+    <t>type="page" subtype="credit" or subtype-"debit"</t>
   </si>
 </sst>
 </file>
@@ -526,12 +535,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -555,12 +570,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -841,10 +858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z79"/>
+  <dimension ref="A1:Z80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D32" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -908,36 +925,36 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="4" t="s">
+    </row>
+    <row r="3" spans="1:26" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>18</v>
+      <c r="E3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -948,33 +965,33 @@
         <v>9</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -982,523 +999,529 @@
         <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>36</v>
+    </row>
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>40</v>
+        <v>33</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" t="s">
-        <v>112</v>
+        <v>45</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>52</v>
+        <v>46</v>
+      </c>
+      <c r="D16" t="s">
+        <v>110</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>54</v>
-      </c>
       <c r="E17" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="B18" s="4" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>65</v>
+        <v>59</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" t="s">
-        <v>113</v>
+        <v>63</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>75</v>
+        <v>38</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" t="s">
+        <v>111</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="D25" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B26" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F26" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B28" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="E29" t="s">
         <v>79</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E28" t="s">
-        <v>81</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C29" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>86</v>
+      <c r="F29" s="4" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C30" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C31" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C32" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
+      <c r="C33" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>96</v>
-      </c>
-      <c r="B34" t="s">
-        <v>99</v>
-      </c>
       <c r="C34" s="4"/>
-      <c r="D34" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E34" t="s">
-        <v>17</v>
-      </c>
-      <c r="F34" t="s">
-        <v>103</v>
-      </c>
+      <c r="D34" s="4"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B35" t="s">
-        <v>90</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="C35" s="4"/>
       <c r="D35" s="4" t="s">
         <v>100</v>
       </c>
       <c r="E35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F35" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B36" t="s">
-        <v>91</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F36" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B37" t="s">
-        <v>92</v>
-      </c>
-      <c r="C37" t="s">
-        <v>94</v>
-      </c>
-      <c r="D37" t="s">
-        <v>98</v>
+        <v>89</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>99</v>
       </c>
       <c r="E37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F37" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>94</v>
+      </c>
+      <c r="B38" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" t="s">
         <v>96</v>
       </c>
-      <c r="B38" t="s">
-        <v>95</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>118</v>
+      <c r="E38" t="s">
+        <v>16</v>
       </c>
       <c r="F38" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B39" t="s">
         <v>93</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E39" t="s">
-        <v>17</v>
+        <v>104</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="F39" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
+      <c r="A40" t="s">
+        <v>94</v>
+      </c>
+      <c r="B40" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E40" t="s">
+        <v>16</v>
+      </c>
+      <c r="F40" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>123</v>
-      </c>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>119</v>
+        <v>7</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>17</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1506,10 +1529,10 @@
         <v>7</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>123</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1517,10 +1540,10 @@
         <v>7</v>
       </c>
       <c r="B44" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E44" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1528,10 +1551,10 @@
         <v>7</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>81</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1539,10 +1562,10 @@
         <v>7</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1550,10 +1573,10 @@
         <v>7</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1561,10 +1584,10 @@
         <v>7</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>135</v>
+        <v>79</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1572,10 +1595,10 @@
         <v>7</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>17</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1583,10 +1606,10 @@
         <v>7</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1594,10 +1617,10 @@
         <v>7</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="E51" t="s">
-        <v>136</v>
+        <v>126</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1605,10 +1628,10 @@
         <v>7</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E52" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1616,10 +1639,10 @@
         <v>7</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E53" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1627,10 +1650,10 @@
         <v>7</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E54" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1638,10 +1661,10 @@
         <v>7</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>138</v>
+        <v>130</v>
+      </c>
+      <c r="E55" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1649,9 +1672,9 @@
         <v>7</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="E56" t="s">
+        <v>131</v>
+      </c>
+      <c r="E56" s="4" t="s">
         <v>136</v>
       </c>
     </row>
@@ -1660,21 +1683,21 @@
         <v>7</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>123</v>
+        <v>135</v>
+      </c>
+      <c r="E57" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1682,10 +1705,10 @@
         <v>7</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1693,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1704,10 +1727,10 @@
         <v>7</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1715,10 +1738,10 @@
         <v>7</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1726,10 +1749,10 @@
         <v>7</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1737,10 +1760,10 @@
         <v>7</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>40</v>
+        <v>133</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1748,10 +1771,10 @@
         <v>7</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1759,10 +1782,10 @@
         <v>7</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>44</v>
+        <v>143</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1770,10 +1793,10 @@
         <v>7</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>146</v>
+        <v>42</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>135</v>
+        <v>38</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1781,10 +1804,10 @@
         <v>7</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>40</v>
+        <v>133</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1792,10 +1815,10 @@
         <v>7</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>123</v>
+        <v>38</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1803,10 +1826,10 @@
         <v>7</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1814,10 +1837,10 @@
         <v>7</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>17</v>
+        <v>121</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1825,10 +1848,10 @@
         <v>7</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>123</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1836,10 +1859,10 @@
         <v>7</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1847,10 +1870,10 @@
         <v>7</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>17</v>
+        <v>133</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1858,10 +1881,10 @@
         <v>7</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1869,10 +1892,10 @@
         <v>7</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>123</v>
+        <v>16</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1880,10 +1903,10 @@
         <v>7</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1891,10 +1914,10 @@
         <v>7</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>17</v>
+        <v>121</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1902,10 +1925,21 @@
         <v>7</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>123</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>